<commit_message>
muda template de alteração do inventário
</commit_message>
<xml_diff>
--- a/ALTERAÇÃO DE PERÍMETRO.xlsx
+++ b/ALTERAÇÃO DE PERÍMETRO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\inventory_change_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7D1FFB-C963-4130-A241-32EBA3CEBDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82E4DA9-EB53-473A-A6C5-A2ABCBDFFF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22410" yWindow="1905" windowWidth="16200" windowHeight="9360" xr2:uid="{05F3C5E2-8288-407C-9DCA-40373417AF91}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{05F3C5E2-8288-407C-9DCA-40373417AF91}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -61,10 +61,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +105,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -107,6 +140,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5802298D-A5A1-4A91-8212-4224A5792C0E}" name="Tabela2" displayName="Tabela2" ref="A1:C200" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C200" xr:uid="{5802298D-A5A1-4A91-8212-4224A5792C0E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{50356129-411A-4E0C-8237-F47A1E838743}" name="Código"/>
+    <tableColumn id="2" xr3:uid="{D3C8876C-22C6-4764-AD4C-71FDDC6DF93E}" name="Id Equipamento"/>
+    <tableColumn id="3" xr3:uid="{F4A8A6FA-6AFA-42C1-A7AF-93204932D7A7}" name="Estação"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,31 +451,1229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E4B02E-3364-48A4-8353-D8704FBEF3C7}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E148" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E149" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E150" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E152" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E153" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E154" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E155" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E156" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E157" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E158" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E159" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E160" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E161" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E162" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E163" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E164" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E165" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E166" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E167" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E168" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E169" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E170" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E171" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E172" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E173" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E174" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E175" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E176" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E177" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E179" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E180" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E181" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E182" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E183" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E184" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E185" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E186" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E187" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E188" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E189" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E190" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E191" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E192" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E193" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E194" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E195" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E196" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E197" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E198" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E199" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E200" s="2" t="str">
+        <f>IF(NOT(OR(ISNUMBER(Tabela2[[#This Row],[Código]]),ISBLANK(Tabela2[[#This Row],[Código]]))),"CAMPO CÓDIGO DEVE SER NÚMERICO", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Id Equipamento]]))),"CAMPO ID EQUIPAMENTO NÃO PODE CONTER ESPAÇOS", IF(NOT(ISERROR(FIND(" ",Tabela2[[#This Row],[Estação]]))),"CAMPO ESTAÇÃO NÃO PODE CONTER ESPAÇOS", "")))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>